<commit_message>
Se agrega modulo para graficar
</commit_message>
<xml_diff>
--- a/pacientes.xlsx
+++ b/pacientes.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB12EEE7-C33A-45C2-A066-22A96CD8F124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>1</t>
   </si>
@@ -23,14 +29,84 @@
   </si>
   <si>
     <t>123456789</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Fernanda</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ID_doctor</t>
+  </si>
+  <si>
+    <t>Altura</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Pulso</t>
+  </si>
+  <si>
+    <t>Peso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -54,23 +130,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -112,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -144,9 +254,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,6 +306,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -353,37 +499,278 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C2" s="1">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="E2" s="1">
         <v>70</v>
       </c>
-      <c r="F1">
-        <v>1.7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F2" s="7">
+        <v>170</v>
+      </c>
+      <c r="G2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>156163132</v>
+      </c>
+      <c r="E3" s="1">
+        <v>85</v>
+      </c>
+      <c r="F3" s="7">
+        <v>185</v>
+      </c>
+      <c r="G3" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2">
+        <v>846541655</v>
+      </c>
+      <c r="E4" s="1">
+        <v>80</v>
+      </c>
+      <c r="F4" s="7">
+        <v>170</v>
+      </c>
+      <c r="G4" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>324684964</v>
+      </c>
+      <c r="E5" s="3">
+        <v>88.3333333333333</v>
+      </c>
+      <c r="F5" s="7">
+        <v>190</v>
+      </c>
+      <c r="G5" s="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2">
+        <v>684684867</v>
+      </c>
+      <c r="E6" s="3">
+        <v>93.3333333333333</v>
+      </c>
+      <c r="F6" s="7">
+        <v>165</v>
+      </c>
+      <c r="G6" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2">
+        <v>464132165</v>
+      </c>
+      <c r="E7" s="3">
+        <v>98.3333333333333</v>
+      </c>
+      <c r="F7" s="7">
+        <v>175</v>
+      </c>
+      <c r="G7" s="1">
+        <v>151.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>65</v>
+      </c>
+      <c r="D8" s="2">
+        <v>464878777</v>
+      </c>
+      <c r="E8" s="3">
+        <v>103.333333333333</v>
+      </c>
+      <c r="F8" s="7">
+        <v>174</v>
+      </c>
+      <c r="G8" s="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2">
+        <v>776454668</v>
+      </c>
+      <c r="E9" s="3">
+        <v>108.333333333333</v>
+      </c>
+      <c r="F9" s="7">
+        <v>174</v>
+      </c>
+      <c r="G9" s="1">
+        <v>154.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>80</v>
+      </c>
+      <c r="D10" s="2">
+        <v>784635123</v>
+      </c>
+      <c r="E10" s="3">
+        <v>113.333333333333</v>
+      </c>
+      <c r="F10" s="7">
+        <v>173</v>
+      </c>
+      <c r="G10" s="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2">
+        <v>862351553</v>
+      </c>
+      <c r="E11" s="3">
+        <v>118.333333333333</v>
+      </c>
+      <c r="F11" s="7">
+        <v>173</v>
+      </c>
+      <c r="G11" s="1">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L17" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se modifica grafico excel, pacientes.xlsx para tomar solo los datos del pulso
</commit_message>
<xml_diff>
--- a/pacientes.xlsx
+++ b/pacientes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Desktop\5to semestre\Progra III\client_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB12EEE7-C33A-45C2-A066-22A96CD8F124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295BF97B-083A-4353-ADAA-3C92C123FC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>1</t>
   </si>
@@ -29,33 +29,6 @@
   </si>
   <si>
     <t>123456789</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Fernanda</t>
-  </si>
-  <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Antonio</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>Pedro</t>
   </si>
   <si>
     <t>ID</t>
@@ -149,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -162,6 +135,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,42 +474,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -558,13 +533,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3" s="8"/>
       <c r="C3" s="1">
         <v>18</v>
       </c>
@@ -581,13 +554,11 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B4" s="8"/>
       <c r="C4" s="1">
         <v>22</v>
       </c>
@@ -604,13 +575,11 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B5" s="8"/>
       <c r="C5" s="1">
         <v>20</v>
       </c>
@@ -627,13 +596,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="1">
         <v>26</v>
       </c>
@@ -650,13 +617,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="1">
         <v>32</v>
       </c>
@@ -673,13 +638,11 @@
         <v>151.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="1">
         <v>65</v>
       </c>
@@ -696,13 +659,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="1">
         <v>50</v>
       </c>
@@ -718,22 +679,21 @@
       <c r="G9" s="1">
         <v>154.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="1">
         <v>80</v>
       </c>
       <c r="D10" s="2">
         <v>784635123</v>
       </c>
-      <c r="E10" s="3">
-        <v>113.333333333333</v>
+      <c r="E10" s="1">
+        <v>85</v>
       </c>
       <c r="F10" s="7">
         <v>173</v>
@@ -742,21 +702,19 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B11" s="8"/>
       <c r="C11" s="1">
         <v>22</v>
       </c>
       <c r="D11" s="2">
         <v>862351553</v>
       </c>
-      <c r="E11" s="3">
-        <v>118.333333333333</v>
+      <c r="E11" s="1">
+        <v>80</v>
       </c>
       <c r="F11" s="7">
         <v>173</v>
@@ -765,8 +723,97 @@
         <v>157.5</v>
       </c>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="8"/>
+      <c r="E12" s="3">
+        <v>88.3333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
+      <c r="E13" s="3">
+        <v>128.333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="8"/>
+      <c r="E14" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="E15" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="8"/>
+      <c r="E16" s="3">
+        <v>88.3333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="8"/>
+      <c r="E17" s="3">
+        <v>70</v>
+      </c>
       <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
+      <c r="E18" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="8"/>
+      <c r="C19" s="6"/>
+      <c r="E19" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+      <c r="E20" s="3">
+        <v>88.3333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="8"/>
+      <c r="E21" s="3">
+        <v>93.3333333333333</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="8"/>
+      <c r="E22" s="3">
+        <v>98.3333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="8"/>
+      <c r="E23" s="3">
+        <v>103.333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="8"/>
+      <c r="E24" s="3">
+        <v>108.333333333333</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="8"/>
+      <c r="E25" s="3">
+        <v>113.333333333333</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="8"/>
+      <c r="E26" s="3">
+        <v>118.333333333333</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>